<commit_message>
Added a call to the JSON endpoint on my local machine.
</commit_message>
<xml_diff>
--- a/data/TestLogs.xlsx
+++ b/data/TestLogs.xlsx
@@ -495,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J260"/>
+  <dimension ref="A1:J286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -10125,6 +10125,968 @@
         </is>
       </c>
       <c r="G260" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D261" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>04/29/2025 14:34:09</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B262" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C262" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D262" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E262" s="2" t="inlineStr">
+        <is>
+          <t>04/29/2025 14:34:36</t>
+        </is>
+      </c>
+      <c r="F262" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G262" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D263" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>04/29/2025 14:36:44</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B264" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C264" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D264" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E264" s="2" t="inlineStr">
+        <is>
+          <t>04/29/2025 14:37:11</t>
+        </is>
+      </c>
+      <c r="F264" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G264" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D265" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>04/29/2025 15:10:18</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B266" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C266" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D266" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E266" s="2" t="inlineStr">
+        <is>
+          <t>04/29/2025 15:10:45</t>
+        </is>
+      </c>
+      <c r="F266" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G266" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D267" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:44:31</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B268" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C268" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D268" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E268" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:44:57</t>
+        </is>
+      </c>
+      <c r="F268" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G268" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D269" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:46:30</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B270" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C270" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D270" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E270" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:46:58</t>
+        </is>
+      </c>
+      <c r="F270" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G270" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D271" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:49:35</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B272" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C272" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D272" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E272" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:49:48</t>
+        </is>
+      </c>
+      <c r="F272" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G272" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D273" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:58:19</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B274" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C274" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D274" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E274" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 10:58:47</t>
+        </is>
+      </c>
+      <c r="F274" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G274" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D275" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:01:29</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B276" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C276" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D276" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E276" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:01:59</t>
+        </is>
+      </c>
+      <c r="F276" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G276" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D277" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:03:38</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B278" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C278" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D278" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E278" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:04:03</t>
+        </is>
+      </c>
+      <c r="F278" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G278" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D279" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:04:44</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B280" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C280" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D280" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E280" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:05:19</t>
+        </is>
+      </c>
+      <c r="F280" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G280" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D281" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:17:26</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B282" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C282" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D282" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E282" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:18:02</t>
+        </is>
+      </c>
+      <c r="F282" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G282" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D283" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:23:35</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B284" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C284" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D284" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E284" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:24:01</t>
+        </is>
+      </c>
+      <c r="F284" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G284" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>navigate</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+      <c r="D285" s="3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:25:09</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Navigating to base URL</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>https://automationpanda.com/2021/12/29/want-to-practice-test-automation-try-these-demo-sites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="2" t="inlineStr">
+        <is>
+          <t>Close Driver</t>
+        </is>
+      </c>
+      <c r="B286" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="C286" s="2" t="inlineStr">
+        <is>
+          <t>n/a</t>
+        </is>
+      </c>
+      <c r="D286" s="2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="E286" s="2" t="inlineStr">
+        <is>
+          <t>04/30/2025 11:25:40</t>
+        </is>
+      </c>
+      <c r="F286" s="2" t="inlineStr">
+        <is>
+          <t>Closing Driver</t>
+        </is>
+      </c>
+      <c r="G286" s="2" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>

</xml_diff>